<commit_message>
Big update for 2026GR, including the rest of the changes for ODS 1.7; new logo
</commit_message>
<xml_diff>
--- a/files/Stembureaus Open Data Standaard 1.7 - gemeenteraadsverkiezingen 2026 voorbeeld.xlsx
+++ b/files/Stembureaus Open Data Standaard 1.7 - gemeenteraadsverkiezingen 2026 voorbeeld.xlsx
@@ -38,7 +38,7 @@
     <t xml:space="preserve">Op het tabblad 'Attributen' staan alle attributen die voor elk stembureau toepasbaar zijn.
 De kolommen 'Opmerkingen, 'Format' en 'Voorbeeld' geven meer informatie over het attribuut. De 'Opmerkingen'-kolom geeft algemene informatie over het attribuut en geeft soms meer informatie over hoe u het veld moet gebruiken zoals gespecificeerd in de 'Format'-kolom. In de 'Voorbeeld'-kolom wordt een voorbeeld gegeven van hoe u het attribuut moet gebruiken.
 Sommige gemeenten werken met mobiele stembureaus die gedurende de dag op verschillende locaties staan. Voor mobiele stembureaus moeten alle attributen voor elke locatie apart worden ingevoerd.
-Sommige toegankelijkheidsattributen zijn niet gedurende de hele openingstijd van een stembureau beschikbaar. Bijvoorbeeld een 'Gebarentolk (NGT)' met de waarde 'op locatie', die gedurende de dag langs meerdere stembureaus gaat. Vul deze informatie dan in het 'Extra toegankelijkheidsinformatie'-attribuut in, bijvoorbeeld: 'Gebarentolk op locatie (NGT) is aanwezig van 10:00-12:00 en 16:00-18:00'.</t>
+Sommige toegankelijkheidsattributen kunnen soms niet gedurende de hele openingstijd van een stembureau beschikbaar zijn. Bijvoorbeeld een 'Gebarentolk (NGT)' met de waarde 'op locatie', die gedurende de dag langs meerdere stembureaus gaat. Vul deze informatie dan in het 'Extra toegankelijkheidsinformatie'-attribuut in, bijvoorbeeld: 'Gebarentolk op locatie (NGT) is aanwezig van 10:00-12:00 en 16:00-18:00'.</t>
   </si>
   <si>
     <t xml:space="preserve">Metadata</t>
@@ -1934,7 +1934,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>